<commit_message>
improve quality of querymodel testarc
</commit_message>
<xml_diff>
--- a/tests/ARCtrl.Querymodel.Tests/TestObjects/TestArc/assays/MS_Cold/isa.assay.xlsx
+++ b/tests/ARCtrl.Querymodel.Tests/TestObjects/TestArc/assays/MS_Cold/isa.assay.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1DFECD6-BCC6-49E3-B600-4AFDCFB73EC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7660A90-04C2-42E2-A46F-B9FD23DD4B7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="930" yWindow="1540" windowWidth="18000" windowHeight="11170" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="isa_assay" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="51">
   <si>
     <t>ASSAY</t>
   </si>
@@ -111,21 +111,9 @@
     <t>Term Accession Number (MS:1001808)</t>
   </si>
   <si>
-    <t>Parameter [injection volume]</t>
-  </si>
-  <si>
     <t>Unit</t>
   </si>
   <si>
-    <t xml:space="preserve">Term Source REF ()  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Term Accession Number ()  </t>
-  </si>
-  <si>
-    <t>user-specific</t>
-  </si>
-  <si>
     <t>Co1_prep</t>
   </si>
   <si>
@@ -166,6 +154,21 @@
   </si>
   <si>
     <t>microliter</t>
+  </si>
+  <si>
+    <t>UO</t>
+  </si>
+  <si>
+    <t>Parameter [injection volume setting]</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Term Source REF (AFR:0001577)  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Term Accession Number (AFR:0001577)  </t>
   </si>
 </sst>
 </file>
@@ -175,10 +178,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00\ &quot;microliter&quot;"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -201,14 +212,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
@@ -254,10 +268,10 @@
     <tableColumn id="9" xr3:uid="{FE989BEA-76F5-4C1C-AED3-42B8FDF2344B}" name="Parameter [technical replicate]" dataDxfId="6"/>
     <tableColumn id="10" xr3:uid="{0466DFAD-77CC-455B-92D9-828B9E54ED9C}" name="Term Source REF (MS:1001808)" dataDxfId="5"/>
     <tableColumn id="11" xr3:uid="{C296C312-9517-4D88-9584-E14DF2DCA0AC}" name="Term Accession Number (MS:1001808)" dataDxfId="4"/>
-    <tableColumn id="21" xr3:uid="{8CB61081-0600-44D2-A13F-ABFEC0CEFA0A}" name="Parameter [injection volume]" dataDxfId="3"/>
+    <tableColumn id="21" xr3:uid="{8CB61081-0600-44D2-A13F-ABFEC0CEFA0A}" name="Parameter [injection volume setting]" dataDxfId="3"/>
     <tableColumn id="22" xr3:uid="{94CAB0F1-3C20-436B-8D49-0B98E6292E1B}" name="Unit" dataDxfId="2"/>
-    <tableColumn id="23" xr3:uid="{85983182-9B6C-4B03-86E9-9DD495F738D0}" name="Term Source REF ()  " dataDxfId="1"/>
-    <tableColumn id="24" xr3:uid="{C39A33DC-9AD3-47AB-85BA-D14EAB1CDD5E}" name="Term Accession Number ()  " dataDxfId="0"/>
+    <tableColumn id="23" xr3:uid="{85983182-9B6C-4B03-86E9-9DD495F738D0}" name="Term Source REF (AFR:0001577)  " dataDxfId="1"/>
+    <tableColumn id="24" xr3:uid="{C39A33DC-9AD3-47AB-85BA-D14EAB1CDD5E}" name="Term Accession Number (AFR:0001577)  " dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{C5872B07-FE34-4D24-ABA3-E118B3FFDC2C}" name="Output [Raw Data File]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -724,10 +738,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DD63E2E-1F83-4137-B747-F3D0805FCBF5}">
-  <dimension ref="A1:AG7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -745,7 +759,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B1" t="s">
         <v>28</v>
@@ -757,181 +771,171 @@
         <v>30</v>
       </c>
       <c r="E1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" t="s">
         <v>31</v>
       </c>
-      <c r="F1" t="s">
-        <v>32</v>
-      </c>
       <c r="G1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="H1" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="I1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" t="s">
-        <v>35</v>
-      </c>
       <c r="E2" s="1">
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G2" t="s">
-        <v>35</v>
+        <v>46</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="I2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" t="s">
-        <v>35</v>
-      </c>
       <c r="E3" s="1">
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G3" t="s">
-        <v>35</v>
+        <v>46</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="I3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" t="s">
-        <v>35</v>
-      </c>
       <c r="E4" s="1">
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G4" t="s">
-        <v>35</v>
+        <v>46</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="I4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" t="s">
-        <v>35</v>
-      </c>
       <c r="E5" s="1">
         <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I5" t="s">
         <v>35</v>
-      </c>
-      <c r="I5" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" t="s">
-        <v>35</v>
-      </c>
       <c r="E6" s="1">
         <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G6" t="s">
-        <v>35</v>
+        <v>46</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="I6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" t="s">
-        <v>35</v>
-      </c>
       <c r="E7" s="1">
         <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G7" t="s">
-        <v>35</v>
+        <v>46</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="I7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{0CC598DB-8391-441C-88F8-ED18DFFFB910}"/>
+    <hyperlink ref="H7" r:id="rId2" xr:uid="{CEA344DE-B499-49AE-A8EA-456FF531472A}"/>
+    <hyperlink ref="H6" r:id="rId3" xr:uid="{3B7D3B79-9352-4737-9253-F9EACF46BA9A}"/>
+    <hyperlink ref="H4" r:id="rId4" xr:uid="{DD294269-CBFF-43E2-9053-490AAB9A7F1F}"/>
+    <hyperlink ref="H5" r:id="rId5" xr:uid="{EE69E281-5627-4139-8DB6-F632F567B1A3}"/>
+    <hyperlink ref="H3" r:id="rId6" xr:uid="{F94842F4-E05C-4317-B107-19A4A8E9F10D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update Querymodel ARCtrl reference
</commit_message>
<xml_diff>
--- a/tests/ARCtrl.Querymodel.Tests/TestObjects/TestArc/assays/MS_Cold/isa.assay.xlsx
+++ b/tests/ARCtrl.Querymodel.Tests/TestObjects/TestArc/assays/MS_Cold/isa.assay.xlsx
@@ -1,18 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF5F7B9-12FB-4536-A44D-30E1B62529F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="isa_assay" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="MS" state="visible" r:id="rId5"/>
+    <sheet name="isa_assay" sheetId="1" r:id="rId1"/>
+    <sheet name="MS_Cold" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="56">
   <si>
     <t>ASSAY</t>
   </si>
@@ -177,19 +181,22 @@
   </si>
   <si>
     <t>Co3_measured</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -216,7 +223,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -232,8 +239,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="annotationTable" displayName="annotationTable" ref="A1:I7" totalsRowShown="1" headerRowCount="1">
-  <autoFilter ref="A1:I7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="annotationTable" displayName="annotationTable" ref="A1:I7">
+  <autoFilter ref="A1:I7" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -245,15 +252,15 @@
     <filterColumn colId="8" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="1" name="Input [Sample Name]" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Parameter [technical replicate]" totalsRowFunction="none"/>
-    <tableColumn id="3" name="Term Source REF (MS:1001808)" totalsRowFunction="none"/>
-    <tableColumn id="4" name="Term Accession Number (MS:1001808)" totalsRowFunction="none"/>
-    <tableColumn id="5" name="Parameter [injection volume setting]" totalsRowFunction="none"/>
-    <tableColumn id="6" name="Unit" totalsRowFunction="none"/>
-    <tableColumn id="7" name="Term Source REF (AFR:0001577)" totalsRowFunction="none"/>
-    <tableColumn id="8" name="Term Accession Number (AFR:0001577)" totalsRowFunction="none"/>
-    <tableColumn id="9" name="Output [Raw Data File]" totalsRowFunction="none"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Input [Sample Name]" totalsRowLabel="Total"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Parameter [technical replicate]"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Term Source REF (MS:1001808)"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Term Accession Number (MS:1001808)"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Parameter [injection volume setting]"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Unit"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Term Source REF (AFR:0001577)"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Term Accession Number (AFR:0001577)"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Output [Raw Data File]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -555,11 +562,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B21"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -628,37 +638,37 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -690,14 +700,19 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:I45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -902,9 +917,14 @@
         <v>54</v>
       </c>
     </row>
+    <row r="45" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I45" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>